<commit_message>
Update de problemas (de nuevo)
</commit_message>
<xml_diff>
--- a/Problemas.xlsx
+++ b/Problemas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProyectosP\Estadistica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D6B95C-74EF-422E-96D7-DAE296EF7C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F110A26-5DEB-4013-BDEF-2F256F552123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respuestas de formulario 1" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="205">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -829,6 +829,12 @@
   </si>
   <si>
     <t>Límite superior (𝜇 + 2𝜎)</t>
+  </si>
+  <si>
+    <t>Rango Edad</t>
+  </si>
+  <si>
+    <t>Densidad</t>
   </si>
 </sst>
 </file>
@@ -937,7 +943,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -977,12 +983,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1210,7 +1210,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1334,21 +1334,6 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1748,7 +1733,1016 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-PA" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Distribución Normal</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-PA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.31926377952755908"/>
+          <c:y val="2.3148148148148147E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PA"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'[Examen de Estadistica Abilio.xlsx]Problema 1'!$F$2:$F$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>4.4991745078873435E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2474670582876769E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.929759876125338E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.4922464390759493E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.8868938668008722E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0781911545247184E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.048418583330622E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.8003551058392009E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.3568505202991663E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.7573536934049048E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0521277669051776E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.2953271149813364E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.5382512232876369E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.8239148095296731E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.1836600062974283E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.63602129664202E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.1875814053049397E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.3523431512623411E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.6914611034999318E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.7575928353725326E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.4036219958073262E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.4896804687108758E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.9452108402753689E-4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.2042546950466716E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredCategoryTitle>
+                <c15:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'[Examen de Estadistica Abilio.xlsx]Problema 1'!$E$2:$E$25</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="24"/>
+                      <c:pt idx="0">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>31</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>37</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>39</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>41</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>42</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c15:cat>
+              </c15:filteredCategoryTitle>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3F83-48CE-ACD9-4B415964BC8E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="73785120"/>
+        <c:axId val="73774560"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="73785120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="73774560"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="73774560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="73785120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-PA"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-PA" sz="1000" b="1" i="0" u="none" strike="noStrike" cap="all" baseline="0"/>
+              <a:t>Distribución Normal de Edades</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1000"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1490693350831146"/>
+          <c:y val="2.3148148148148147E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PA"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'[Examen de Estadistica Abilio.xlsx]Hoja2'!$G$2:$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>9.2026333188312739E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2974958544936327E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7724351072627209E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3458768633597877E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.008226854150443E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.7375452498260561E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.4991745078873435E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.2474670582876769E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.929759876125338E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.4922464390759493E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.8868938668008722E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.0781911545247184E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.048418583330622E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.8003551058392009E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.3568505202991663E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.7573536934049048E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.0521277669051776E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.2953271149813364E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.5382512232876369E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.8239148095296731E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.1836600062974283E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.63602129664202E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.1875814053049397E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.3523431512623411E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'[Examen de Estadistica Abilio.xlsx]Hoja2'!$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Densidad</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredCategoryTitle>
+                <c15:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'[Examen de Estadistica Abilio.xlsx]Hoja2'!$F$2:$F$25</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="24"/>
+                      <c:pt idx="0">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>31</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>36</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c15:cat>
+              </c15:filteredCategoryTitle>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D527-4965-A2A7-48E927F2AD52}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="619555040"/>
+        <c:axId val="619557440"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="619555040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="32000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+            <a:tailEnd type="none" w="med" len="lg"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="619557440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="619557440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="32000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+            <a:tailEnd type="none" w="med" len="lg"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="619555040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-PA"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2307,6 +3301,1035 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="237">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+        <a:tailEnd type="none" w="med" len="lg"/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+        <a:tailEnd type="none" w="med" len="lg"/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="rnd"/>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+        <a:tailEnd type="none" w="med" len="lg"/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2343,6 +4366,138 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>678180</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10A14ECD-007F-4813-5B6A-54B6D6F5E83A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{101F84E6-C304-319F-EC72-3D5918784610}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>12698</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3BB4E64-F8FC-60F9-B855-3F9F5C2A251B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="419100" y="4229100"/>
+          <a:ext cx="5933438" cy="1112520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2583,8 +4738,8 @@
   </sheetPr>
   <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
@@ -6714,7 +8869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22D19530-00BF-4088-B53D-498235A4457A}">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="I76" sqref="I76"/>
     </sheetView>
   </sheetViews>
@@ -7868,7 +10023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE630DB-FFE5-404A-A1EA-9DED0F25390C}">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0"/>
+    <sheetView topLeftCell="A26" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -8587,579 +10742,688 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I31"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" t="s">
         <v>187</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" t="s">
         <v>188</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" t="s">
         <v>189</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" t="s">
         <v>190</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="52">
+      <c r="A2">
         <v>20</v>
       </c>
-      <c r="B2" s="51">
-        <v>24.366666666666667</v>
-      </c>
-      <c r="C2" s="52">
-        <v>5.624253036823843</v>
-      </c>
-      <c r="E2" s="52">
+      <c r="B2">
+        <v>24.3666667</v>
+      </c>
+      <c r="C2">
+        <v>5.6242530369999999</v>
+      </c>
+      <c r="E2">
         <v>19</v>
       </c>
-      <c r="F2" s="52">
-        <v>4.4991745078873435E-2</v>
-      </c>
-      <c r="G2" s="52">
-        <v>0.84173508986374146</v>
-      </c>
-      <c r="H2" s="52">
-        <v>0.54482914892255896</v>
+      <c r="F2">
+        <v>4.4991745E-2</v>
+      </c>
+      <c r="G2">
+        <v>0.84173509000000002</v>
+      </c>
+      <c r="H2">
+        <v>0.54482914900000001</v>
       </c>
       <c r="I2">
-        <v>0.84173508986374146</v>
+        <v>0.84173509000000002</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="52">
+      <c r="A3">
         <v>21</v>
       </c>
-      <c r="E3" s="52">
+      <c r="E3">
         <v>20</v>
       </c>
-      <c r="F3" s="52">
-        <v>5.2474670582876769E-2</v>
+      <c r="F3">
+        <v>5.2474671000000001E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="52">
+      <c r="A4">
         <v>20</v>
       </c>
-      <c r="E4" s="52">
+      <c r="E4">
         <v>21</v>
       </c>
-      <c r="F4" s="52">
-        <v>5.929759876125338E-2</v>
+      <c r="F4">
+        <v>5.9297598999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="52">
+      <c r="A5">
         <v>20</v>
       </c>
-      <c r="E5" s="52">
+      <c r="E5">
         <v>22</v>
       </c>
-      <c r="F5" s="52">
-        <v>6.4922464390759493E-2</v>
+      <c r="F5">
+        <v>6.4922463999999999E-2</v>
       </c>
       <c r="H5" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="52">
+      <c r="A6">
         <v>32</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E6">
         <v>23</v>
       </c>
-      <c r="F6" s="52">
-        <v>6.8868938668008722E-2</v>
+      <c r="F6">
+        <v>6.8868939000000004E-2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="52">
+      <c r="A7">
         <v>31</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" t="s">
         <v>193</v>
       </c>
-      <c r="C7" s="55">
+      <c r="C7">
         <v>42</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="52">
+      <c r="E7">
         <v>24</v>
       </c>
-      <c r="F7" s="52">
-        <v>7.0781911545247184E-2</v>
+      <c r="F7">
+        <v>7.0781912000000002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="52">
+      <c r="A8">
         <v>19</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" t="s">
         <v>194</v>
       </c>
-      <c r="C8" s="55">
+      <c r="C8">
         <v>19</v>
       </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="52">
+      <c r="E8">
         <v>25</v>
       </c>
-      <c r="F8" s="52">
-        <v>7.048418583330622E-2</v>
+      <c r="F8">
+        <v>7.0484186000000004E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="52">
+      <c r="A9">
         <v>19</v>
       </c>
-      <c r="E9" s="52">
-        <v>26</v>
-      </c>
-      <c r="F9" s="52">
-        <v>6.8003551058392009E-2</v>
+      <c r="E9">
+        <v>26</v>
+      </c>
+      <c r="F9">
+        <v>6.8003550999999995E-2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="52">
+      <c r="A10">
         <v>20</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E10">
         <v>27</v>
       </c>
-      <c r="F10" s="52">
-        <v>6.3568505202991663E-2</v>
+      <c r="F10">
+        <v>6.3568504999999997E-2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="52">
+      <c r="A11">
         <v>19</v>
       </c>
-      <c r="E11" s="52">
-        <v>28</v>
-      </c>
-      <c r="F11" s="52">
-        <v>5.7573536934049048E-2</v>
+      <c r="E11">
+        <v>28</v>
+      </c>
+      <c r="F11">
+        <v>5.7573537000000001E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="52">
+      <c r="A12">
         <v>20</v>
       </c>
-      <c r="E12" s="52">
+      <c r="E12">
         <v>29</v>
       </c>
-      <c r="F12" s="52">
-        <v>5.0521277669051776E-2</v>
+      <c r="F12">
+        <v>5.0521278000000003E-2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="52">
-        <v>26</v>
-      </c>
-      <c r="E13" s="52">
+      <c r="A13">
+        <v>26</v>
+      </c>
+      <c r="E13">
         <v>30</v>
       </c>
-      <c r="F13" s="52">
-        <v>4.2953271149813364E-2</v>
+      <c r="F13">
+        <v>4.2953271000000001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="52">
+      <c r="A14">
         <v>22</v>
       </c>
-      <c r="E14" s="52">
+      <c r="E14">
         <v>31</v>
       </c>
-      <c r="F14" s="52">
-        <v>3.5382512232876369E-2</v>
+      <c r="F14">
+        <v>3.5382511999999998E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="52">
-        <v>26</v>
-      </c>
-      <c r="E15" s="52">
+      <c r="A15">
+        <v>26</v>
+      </c>
+      <c r="E15">
         <v>32</v>
       </c>
-      <c r="F15" s="52">
-        <v>2.8239148095296731E-2</v>
+      <c r="F15">
+        <v>2.8239147999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="52">
-        <v>28</v>
-      </c>
-      <c r="E16" s="52">
+      <c r="A16">
+        <v>28</v>
+      </c>
+      <c r="E16">
         <v>33</v>
       </c>
-      <c r="F16" s="52">
-        <v>2.1836600062974283E-2</v>
+      <c r="F16">
+        <v>2.1836600000000001E-2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="52">
+      <c r="A17">
         <v>24</v>
       </c>
-      <c r="E17" s="52">
+      <c r="E17">
         <v>34</v>
       </c>
-      <c r="F17" s="52">
-        <v>1.63602129664202E-2</v>
+      <c r="F17">
+        <v>1.6360212999999998E-2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="52">
+      <c r="A18">
         <v>24</v>
       </c>
-      <c r="E18" s="52">
+      <c r="E18">
         <v>35</v>
       </c>
-      <c r="F18" s="52">
-        <v>1.1875814053049397E-2</v>
+      <c r="F18">
+        <v>1.1875814E-2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="52">
+      <c r="A19">
         <v>19</v>
       </c>
-      <c r="E19" s="52">
+      <c r="E19">
         <v>36</v>
       </c>
-      <c r="F19" s="52">
-        <v>8.3523431512623411E-3</v>
+      <c r="F19">
+        <v>8.3523429999999999E-3</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="52">
+      <c r="A20">
         <v>25</v>
       </c>
-      <c r="E20" s="52">
+      <c r="E20">
         <v>37</v>
       </c>
-      <c r="F20" s="52">
-        <v>5.6914611034999318E-3</v>
+      <c r="F20">
+        <v>5.6914610000000001E-3</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="52">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="E21" s="52">
+      <c r="E21">
         <v>38</v>
       </c>
-      <c r="F21" s="52">
-        <v>3.7575928353725326E-3</v>
+      <c r="F21">
+        <v>3.757593E-3</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="52">
+      <c r="A22">
         <v>42</v>
       </c>
-      <c r="E22" s="52">
+      <c r="E22">
         <v>39</v>
       </c>
-      <c r="F22" s="52">
-        <v>2.4036219958073262E-3</v>
+      <c r="F22">
+        <v>2.4036219999999998E-3</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="52">
+      <c r="A23">
         <v>20</v>
       </c>
-      <c r="E23" s="52">
+      <c r="E23">
         <v>40</v>
       </c>
-      <c r="F23" s="52">
-        <v>1.4896804687108758E-3</v>
+      <c r="F23">
+        <v>1.48968E-3</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="52">
-        <v>28</v>
-      </c>
-      <c r="E24" s="52">
-        <v>41</v>
-      </c>
-      <c r="F24" s="52">
-        <v>8.9452108402753689E-4</v>
+      <c r="A24">
+        <v>28</v>
+      </c>
+      <c r="E24">
+        <v>41</v>
+      </c>
+      <c r="F24">
+        <v>8.9452100000000001E-4</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="52">
-        <v>28</v>
-      </c>
-      <c r="E25" s="52">
+      <c r="A25">
+        <v>28</v>
+      </c>
+      <c r="E25">
         <v>42</v>
       </c>
-      <c r="F25" s="52">
-        <v>5.2042546950466716E-4</v>
+      <c r="F25">
+        <v>5.2042500000000003E-4</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="52">
+      <c r="A26">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="52">
+      <c r="A27">
         <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="52">
+      <c r="A28">
         <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="52">
+      <c r="A29">
         <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="52">
+      <c r="A30">
         <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="52">
+      <c r="A31">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7583C22A-DACA-4D83-99FF-95228F8B6234}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" t="s">
         <v>195</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" t="s">
         <v>196</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="52">
+      <c r="F1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>20</v>
       </c>
       <c r="B2">
-        <v>24.366666666666667</v>
-      </c>
-      <c r="C2" s="43">
+        <v>24.366666670000001</v>
+      </c>
+      <c r="C2">
         <v>29</v>
       </c>
-      <c r="D2" s="43">
-        <v>0.96666666666666667</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="52">
+      <c r="D2">
+        <v>0.96666666700000003</v>
+      </c>
+      <c r="F2">
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>9.202633E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>21</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" t="s">
         <v>198</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" t="s">
         <v>199</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="52">
+      <c r="F3">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>1.2974958999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>20</v>
       </c>
       <c r="B4">
-        <v>5.624253036823843</v>
-      </c>
-      <c r="C4" s="43">
+        <v>5.6242530369999999</v>
+      </c>
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="43">
-        <v>3.3333333333333333E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="52">
+      <c r="D4">
+        <v>3.3333333E-2</v>
+      </c>
+      <c r="F4">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>1.7724350999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>20</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="52">
+      <c r="F5">
+        <v>16</v>
+      </c>
+      <c r="G5">
+        <v>2.3458769000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>32</v>
       </c>
       <c r="B6">
-        <v>13.118160593018981</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="52">
+        <v>13.11816059</v>
+      </c>
+      <c r="F6">
+        <v>17</v>
+      </c>
+      <c r="G6">
+        <v>3.0082268999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>31</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="52">
+      <c r="F7">
+        <v>18</v>
+      </c>
+      <c r="G7">
+        <v>3.7375452000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>19</v>
       </c>
       <c r="B8">
-        <v>35.61517274031435</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="52">
+        <v>35.615172739999998</v>
+      </c>
+      <c r="F8">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="52">
+      <c r="G8">
+        <v>4.4991745E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>19</v>
+      </c>
+      <c r="F9">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="52">
+      <c r="G9">
+        <v>5.2474671000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>21</v>
+      </c>
+      <c r="G10">
+        <v>5.9297598999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="52">
+      <c r="F11">
+        <v>22</v>
+      </c>
+      <c r="G11">
+        <v>6.4922463999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="52">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="52">
+      <c r="F12">
+        <v>23</v>
+      </c>
+      <c r="G12">
+        <v>6.8868939000000004E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>26</v>
+      </c>
+      <c r="F13">
+        <v>24</v>
+      </c>
+      <c r="G13">
+        <v>7.0781912000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="52">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="52">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52">
+      <c r="F14">
+        <v>25</v>
+      </c>
+      <c r="G14">
+        <v>7.0484186000000004E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>26</v>
+      </c>
+      <c r="F15">
+        <v>26</v>
+      </c>
+      <c r="G15">
+        <v>6.8003550999999995E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>28</v>
+      </c>
+      <c r="F16">
+        <v>27</v>
+      </c>
+      <c r="G16">
+        <v>6.3568504999999997E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="52">
+      <c r="F17">
+        <v>28</v>
+      </c>
+      <c r="G17">
+        <v>5.7573537000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="52">
+      <c r="F18">
+        <v>29</v>
+      </c>
+      <c r="G18">
+        <v>5.0521278000000003E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="52">
+      <c r="F19">
+        <v>30</v>
+      </c>
+      <c r="G19">
+        <v>4.2953271000000001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="52">
+      <c r="F20">
+        <v>31</v>
+      </c>
+      <c r="G20">
+        <v>3.5382511999999998E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52">
+      <c r="F21">
+        <v>32</v>
+      </c>
+      <c r="G21">
+        <v>2.8239147999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>42</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="52">
+      <c r="F22">
+        <v>33</v>
+      </c>
+      <c r="G22">
+        <v>2.1836600000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="52">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="52">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="52">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="52">
+      <c r="F23">
+        <v>34</v>
+      </c>
+      <c r="G23">
+        <v>1.6360212999999998E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>28</v>
+      </c>
+      <c r="F24">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="52">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="52">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="52">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="52">
-        <v>19</v>
+      <c r="G24">
+        <v>1.1875814E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Anterior antes del nuevo cambio
</commit_message>
<xml_diff>
--- a/Problemas.xlsx
+++ b/Problemas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProyectosP\Estadistica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F110A26-5DEB-4013-BDEF-2F256F552123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4AF23B-7E96-4C44-96A4-66CD4D7FADAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respuestas de formulario 1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="Temas 7 P1" sheetId="6" r:id="rId5"/>
     <sheet name="Tema 7 P2" sheetId="7" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -60,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="234">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -835,6 +838,135 @@
   </si>
   <si>
     <t>Densidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distribuciones probabilisticas </t>
+  </si>
+  <si>
+    <t>Modela las respuestas de la pregunta "¿Qué tan actualizado te consideras?" con una distribución binomial.</t>
+  </si>
+  <si>
+    <t>En una distribución binomial solo existen dos posibles resultados, es por ello que para modelar la pregunta a este sistema, es necesario reducir el número de respuestas posibles a solo 2.</t>
+  </si>
+  <si>
+    <t>"Actualizado" englobaria las respuesta de "Muy actualizado y Bastante actualizado", mientras que "No actualizado" englobaria las respuestas de "Poco actualizado y Nada actualizado"</t>
+  </si>
+  <si>
+    <t>Teniendo esto en cuenta utilizaremos solo la variable de "Actualizado" y así podemos sacar la probabilidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> de los estudiantes que se consideran "Actualizados" y hacer una distribución binomial</t>
+  </si>
+  <si>
+    <t>P(Muy actualizado) =</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">P(Muy actualizado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>∩ Bastante</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) =</t>
+    </r>
+  </si>
+  <si>
+    <t>P(Actualizados) =</t>
+  </si>
+  <si>
+    <t>Encuentra la probabilidad acumulada hasta un nivel intermedio en Blockchain</t>
+  </si>
+  <si>
+    <t>Datos</t>
+  </si>
+  <si>
+    <t>X =</t>
+  </si>
+  <si>
+    <t>Personas con niveles de conocimiento "ninguno, básico e intermedio"</t>
+  </si>
+  <si>
+    <t>n =</t>
+  </si>
+  <si>
+    <t>Tamaño de la muestra</t>
+  </si>
+  <si>
+    <t>P =</t>
+  </si>
+  <si>
+    <t>Probabilidad de éxito</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">P(x </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>≥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 29)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">La probabilidad acumulada P(x ≥ 29) que da como resultado 0.64 indica que de 30 estudiantes encuestados hay un 64% de probabilidad acumulada que al menos 29 estudiantes  </t>
+  </si>
+  <si>
+    <t>tengan un nivel de conocimiento que sea "ninguno", "básico" o "intermedio".</t>
+  </si>
+  <si>
+    <t>Problema 3</t>
+  </si>
+  <si>
+    <t>Supongamos que, en base a las respuestas de la encuesta, se identificó que en promedio 2 estudiantes por carrera tienen un nivel avanzado de conocimiento en IA.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Queremos calcular la probabilidad de que exactamente 3 estudiantes de una carrera tengan este nivel avanzado.</t>
+  </si>
+  <si>
+    <t>Estudiantes con un nivel avanzado en IA</t>
+  </si>
+  <si>
+    <t>media =</t>
+  </si>
+  <si>
+    <t>Promedio de estudiantes por carrera</t>
+  </si>
+  <si>
+    <t>P(x = 3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si seleccionamos una carrera al azar y sabemos que, en promedio, 2 estudiantes tienen un nivel avanzado en IA, </t>
+  </si>
+  <si>
+    <t>hay una probabilidad de 0.18 o 18% de encontrar exactamente 3 estudiantes avanzados en esa carrera.</t>
   </si>
 </sst>
 </file>
@@ -943,7 +1075,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -983,6 +1115,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1204,13 +1348,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1334,11 +1479,32 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{CE4CF6DF-9C20-4C6A-9718-52E302F7CE91}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{5ABA7043-3B48-41C0-AEC3-97CD253758D2}"/>
+    <cellStyle name="Normal 4" xfId="4" xr:uid="{A9012787-2A64-4B08-A60F-11229775AE80}"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="4">
@@ -1767,6 +1933,977 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="es-PA"/>
+              <a:t>Distribución binomial</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PA"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'[Probabilidad y distribuciones.xlsx]Distribuciones probabilísticas'!$B$16:$B$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>3.4494548241361291E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.2267967563358112E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5033352620270574E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.5432311397463387E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.631109148739923E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5883276004222625E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.5106514326435229E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.13318739229617493</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.15640139200976874</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.15615663239785987</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.13394280159196714</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.9470966611191994E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.4329228407003253E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.6381210431696342E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.8044201954553626E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.8615114618900278E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.0103498995793687E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.0125949123688698E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.9870757587094191E-4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.7057254561221336E-5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.7310749440161678E-5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.3669465711917415E-6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.6259478558325731E-7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.9927734387823432E-8</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.5219073243709207E-9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.3341514052988687E-10</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.3318090670007437E-11</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.4365667802404147E-12</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.9415558847128475E-13</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.4691715062333685E-15</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.4462898441675134E-17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredCategoryTitle>
+                <c15:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'[Probabilidad y distribuciones.xlsx]Distribuciones probabilísticas'!$A$16:$A$46</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="31"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>30</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c15:cat>
+              </c15:filteredCategoryTitle>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D598-4391-9594-10A91B9B17E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1449964544"/>
+        <c:axId val="1449965376"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1449964544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1449965376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1449965376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1449964544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-PA"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-PA" sz="1000" b="1" i="0" u="none" strike="noStrike" cap="all" baseline="0"/>
+              <a:t>Distribución Normal de Edades</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1000"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1490693350831146"/>
+          <c:y val="2.3148148148148147E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PA"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10209755030621172"/>
+          <c:y val="0.16898148148148148"/>
+          <c:w val="0.88123578302712158"/>
+          <c:h val="0.75240740740740741"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'[Examen de Estadistica Abilio.xlsx]Hoja2'!$G$2:$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>9.2026333188312739E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2974958544936327E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7724351072627209E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3458768633597877E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.008226854150443E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.7375452498260561E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.4991745078873435E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.2474670582876769E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.929759876125338E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.4922464390759493E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.8868938668008722E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.0781911545247184E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.048418583330622E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.8003551058392009E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.3568505202991663E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.7573536934049048E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.0521277669051776E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.2953271149813364E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.5382512232876369E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.8239148095296731E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.1836600062974283E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.63602129664202E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.1875814053049397E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.3523431512623411E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredSeriesTitle>
+                <c15:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'[Examen de Estadistica Abilio.xlsx]Hoja2'!$G$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Densidad</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:tx>
+              </c15:filteredSeriesTitle>
+            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredCategoryTitle>
+                <c15:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'[Examen de Estadistica Abilio.xlsx]Hoja2'!$F$2:$F$25</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="24"/>
+                      <c:pt idx="0">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>31</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>36</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c15:cat>
+              </c15:filteredCategoryTitle>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8E28-4FE4-882A-642536637CC1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="619555040"/>
+        <c:axId val="619557440"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="619555040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="32000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+            <a:tailEnd type="none" w="med" len="lg"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="619557440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="619557440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="32000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+            <a:tailEnd type="none" w="med" len="lg"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="619555040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-PA"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
               <a:rPr lang="es-PA" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
               <a:t>Distribución Normal</a:t>
             </a:r>
@@ -2007,7 +3144,7 @@
               </c15:filteredCategoryTitle>
             </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3F83-48CE-ACD9-4B415964BC8E}"/>
+              <c16:uniqueId val="{00000000-91D2-4E71-B9E1-F57257AB20D8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2175,493 +3312,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-PA" sz="1000" b="1" i="0" u="none" strike="noStrike" cap="all" baseline="0"/>
-              <a:t>Distribución Normal de Edades</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1000"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.1490693350831146"/>
-          <c:y val="2.3148148148148147E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-PA"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'[Examen de Estadistica Abilio.xlsx]Hoja2'!$G$2:$G$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>9.2026333188312739E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.2974958544936327E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.7724351072627209E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.3458768633597877E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.008226854150443E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.7375452498260561E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.4991745078873435E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.2474670582876769E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.929759876125338E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6.4922464390759493E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6.8868938668008722E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7.0781911545247184E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>7.048418583330622E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.8003551058392009E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6.3568505202991663E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.7573536934049048E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.0521277669051776E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4.2953271149813364E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.5382512232876369E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2.8239148095296731E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.1836600062974283E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.63602129664202E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.1875814053049397E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>8.3523431512623411E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:filteredSeriesTitle>
-                <c15:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>'[Examen de Estadistica Abilio.xlsx]Hoja2'!$G$1</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>Densidad</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c15:tx>
-              </c15:filteredSeriesTitle>
-            </c:ext>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:filteredCategoryTitle>
-                <c15:cat>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>'[Examen de Estadistica Abilio.xlsx]Hoja2'!$F$2:$F$25</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="24"/>
-                      <c:pt idx="0">
-                        <c:v>13</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>14</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>15</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>16</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>17</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>18</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>19</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>20</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>21</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>22</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>23</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>24</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>25</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>26</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>27</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>28</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>29</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>30</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>31</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>32</c:v>
-                      </c:pt>
-                      <c:pt idx="20">
-                        <c:v>33</c:v>
-                      </c:pt>
-                      <c:pt idx="21">
-                        <c:v>34</c:v>
-                      </c:pt>
-                      <c:pt idx="22">
-                        <c:v>35</c:v>
-                      </c:pt>
-                      <c:pt idx="23">
-                        <c:v>36</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c15:cat>
-              </c15:filteredCategoryTitle>
-            </c:ext>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D527-4965-A2A7-48E927F2AD52}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="619555040"/>
-        <c:axId val="619557440"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="619555040"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                  <a:alpha val="32000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-            <a:tailEnd type="none" w="med" len="lg"/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-PA"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="619557440"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="619557440"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                  <a:alpha val="32000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-            <a:tailEnd type="none" w="med" len="lg"/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-PA"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="619555040"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-PA"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2743,6 +3393,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3302,7 +3992,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3410,11 +4100,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -3425,11 +4110,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -3461,9 +4141,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4330,6 +5007,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4373,29 +5566,31 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>678180</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:colOff>716280</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2">
+        <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10A14ECD-007F-4813-5B6A-54B6D6F5E83A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A9E6C98-031D-45D5-8805-859A40EEE376}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4414,29 +5609,31 @@
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Gráfico 3">
+        <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{101F84E6-C304-319F-EC72-3D5918784610}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E08A224F-7B3E-44B5-9E94-83B2703C7175}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4450,6 +5647,11 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -4477,7 +5679,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -4500,7 +5702,61 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB8975D9-6225-41DA-8410-CB10C63F0381}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Hoja1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4738,9 +5994,9 @@
   </sheetPr>
   <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7062,8 +8318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCBC7F30-86F4-4ABF-9E6F-58C578F74CE5}">
   <dimension ref="A4:I140"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+    <sheetView topLeftCell="D46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -8869,8 +10125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22D19530-00BF-4088-B53D-498235A4457A}">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="I76" sqref="I76"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10021,9 +11277,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE630DB-FFE5-404A-A1EA-9DED0F25390C}">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:I157"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A148" sqref="A148"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -10727,13 +11985,743 @@
       <c r="E80" s="44"/>
       <c r="F80" s="44"/>
     </row>
-    <row r="81" spans="1:1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A81" s="44" t="s">
         <v>184</v>
       </c>
     </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A86" s="54" t="s">
+        <v>124</v>
+      </c>
+      <c r="B86" s="54"/>
+      <c r="C86" s="54"/>
+      <c r="D86" s="54"/>
+      <c r="E86" s="54"/>
+      <c r="F86" s="54"/>
+      <c r="G86" s="54"/>
+      <c r="H86" s="54"/>
+      <c r="I86" s="54"/>
+    </row>
+    <row r="87" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A87" s="51" t="s">
+        <v>206</v>
+      </c>
+      <c r="B87" s="51"/>
+      <c r="C87" s="51"/>
+      <c r="D87" s="51"/>
+      <c r="E87" s="51"/>
+      <c r="F87" s="51"/>
+      <c r="G87" s="51"/>
+      <c r="H87" s="51"/>
+      <c r="I87" s="51"/>
+    </row>
+    <row r="89" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A89" s="51" t="s">
+        <v>207</v>
+      </c>
+      <c r="B89" s="51"/>
+      <c r="C89" s="51"/>
+      <c r="D89" s="51"/>
+      <c r="E89" s="51"/>
+      <c r="F89" s="51"/>
+      <c r="G89" s="51"/>
+      <c r="H89" s="51"/>
+      <c r="I89" s="51"/>
+    </row>
+    <row r="90" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A90" s="51" t="s">
+        <v>208</v>
+      </c>
+      <c r="B90" s="51"/>
+      <c r="C90" s="51"/>
+      <c r="D90" s="51"/>
+      <c r="E90" s="51"/>
+      <c r="F90" s="51"/>
+      <c r="G90" s="51"/>
+      <c r="H90" s="51"/>
+      <c r="I90" s="51"/>
+    </row>
+    <row r="92" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A92" s="51" t="s">
+        <v>209</v>
+      </c>
+      <c r="B92" s="51"/>
+      <c r="C92" s="51"/>
+      <c r="D92" s="51"/>
+      <c r="E92" s="51"/>
+      <c r="F92" s="51"/>
+      <c r="G92" s="51"/>
+      <c r="H92" s="51"/>
+      <c r="I92" s="51"/>
+    </row>
+    <row r="93" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A93" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="B93" s="51"/>
+      <c r="C93" s="51"/>
+      <c r="D93" s="51"/>
+      <c r="E93" s="51"/>
+      <c r="F93" s="51"/>
+      <c r="G93" s="51"/>
+      <c r="H93" s="51"/>
+      <c r="I93" s="51"/>
+    </row>
+    <row r="95" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A95" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="B95" s="51"/>
+      <c r="C95" s="51"/>
+      <c r="D95" s="52">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="E95" s="51"/>
+      <c r="F95" s="51"/>
+      <c r="G95" s="51"/>
+      <c r="H95" s="51"/>
+      <c r="I95" s="51"/>
+    </row>
+    <row r="96" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A96" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="B96" s="51"/>
+      <c r="C96" s="51"/>
+      <c r="D96" s="52">
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="E96" s="51"/>
+      <c r="F96" s="51"/>
+      <c r="G96" s="51"/>
+      <c r="H96" s="51"/>
+      <c r="I96" s="51"/>
+    </row>
+    <row r="97" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A97" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="B97" s="51"/>
+      <c r="C97" s="51"/>
+      <c r="D97" s="52">
+        <v>8.8888888888888889E-3</v>
+      </c>
+      <c r="E97" s="51"/>
+      <c r="F97" s="51"/>
+      <c r="G97" s="51"/>
+      <c r="H97" s="51"/>
+      <c r="I97" s="51"/>
+    </row>
+    <row r="98" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A98" s="51" t="s">
+        <v>213</v>
+      </c>
+      <c r="B98" s="51"/>
+      <c r="C98" s="51"/>
+      <c r="D98" s="52">
+        <v>0.2911111111111111</v>
+      </c>
+      <c r="E98" s="51"/>
+      <c r="F98" s="51"/>
+      <c r="G98" s="51"/>
+      <c r="H98" s="51"/>
+      <c r="I98" s="51"/>
+    </row>
+    <row r="101" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A101" s="53">
+        <v>0</v>
+      </c>
+      <c r="B101" s="53">
+        <v>3.4494548241361291E-5</v>
+      </c>
+      <c r="C101" s="51"/>
+      <c r="D101" s="51"/>
+      <c r="E101" s="51"/>
+      <c r="F101" s="51"/>
+      <c r="G101" s="51"/>
+      <c r="H101" s="51"/>
+      <c r="I101" s="51"/>
+    </row>
+    <row r="102" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A102" s="53">
+        <v>1</v>
+      </c>
+      <c r="B102" s="53">
+        <v>4.2267967563358112E-4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A103" s="53">
+        <v>2</v>
+      </c>
+      <c r="B103" s="53">
+        <v>2.5033352620270574E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A104" s="53">
+        <v>3</v>
+      </c>
+      <c r="B104" s="53">
+        <v>9.5432311397463387E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A105" s="53">
+        <v>4</v>
+      </c>
+      <c r="B105" s="53">
+        <v>2.631109148739923E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A106" s="53">
+        <v>5</v>
+      </c>
+      <c r="B106" s="53">
+        <v>5.5883276004222625E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A107" s="53">
+        <v>6</v>
+      </c>
+      <c r="B107" s="53">
+        <v>9.5106514326435229E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A108" s="53">
+        <v>7</v>
+      </c>
+      <c r="B108" s="53">
+        <v>0.13318739229617493</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A109" s="53">
+        <v>8</v>
+      </c>
+      <c r="B109" s="53">
+        <v>0.15640139200976874</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A110" s="53">
+        <v>9</v>
+      </c>
+      <c r="B110" s="53">
+        <v>0.15615663239785987</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A111" s="53">
+        <v>10</v>
+      </c>
+      <c r="B111" s="53">
+        <v>0.13394280159196714</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A112" s="53">
+        <v>11</v>
+      </c>
+      <c r="B112" s="53">
+        <v>9.9470966611191994E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A113" s="53">
+        <v>12</v>
+      </c>
+      <c r="B113" s="53">
+        <v>6.4329228407003253E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A114" s="53">
+        <v>13</v>
+      </c>
+      <c r="B114" s="53">
+        <v>3.6381210431696342E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A115" s="53">
+        <v>14</v>
+      </c>
+      <c r="B115" s="53">
+        <v>1.8044201954553626E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A116" s="53">
+        <v>15</v>
+      </c>
+      <c r="B116" s="53">
+        <v>7.8615114618900278E-3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A117" s="53">
+        <v>16</v>
+      </c>
+      <c r="B117" s="53">
+        <v>3.0103498995793687E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A118" s="53">
+        <v>17</v>
+      </c>
+      <c r="B118" s="53">
+        <v>1.0125949123688698E-3</v>
+      </c>
+      <c r="C118" s="51"/>
+      <c r="D118" s="51"/>
+      <c r="E118" s="51"/>
+      <c r="F118" s="51"/>
+      <c r="G118" s="51"/>
+      <c r="H118" s="51"/>
+      <c r="I118" s="51"/>
+    </row>
+    <row r="119" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A119" s="53">
+        <v>18</v>
+      </c>
+      <c r="B119" s="53">
+        <v>2.9870757587094191E-4</v>
+      </c>
+      <c r="C119" s="51"/>
+      <c r="D119" s="51"/>
+      <c r="E119" s="51"/>
+      <c r="F119" s="51"/>
+      <c r="G119" s="51"/>
+      <c r="H119" s="51"/>
+      <c r="I119" s="51"/>
+    </row>
+    <row r="120" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A120" s="53">
+        <v>19</v>
+      </c>
+      <c r="B120" s="53">
+        <v>7.7057254561221336E-5</v>
+      </c>
+      <c r="C120" s="51"/>
+      <c r="D120" s="51"/>
+      <c r="E120" s="51"/>
+      <c r="F120" s="51"/>
+      <c r="G120" s="51"/>
+      <c r="H120" s="51"/>
+      <c r="I120" s="51"/>
+    </row>
+    <row r="121" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A121" s="53">
+        <v>20</v>
+      </c>
+      <c r="B121" s="53">
+        <v>1.7310749440161678E-5</v>
+      </c>
+      <c r="C121" s="51"/>
+      <c r="D121" s="51"/>
+      <c r="E121" s="51"/>
+      <c r="F121" s="51"/>
+      <c r="G121" s="51"/>
+      <c r="H121" s="51"/>
+      <c r="I121" s="51"/>
+    </row>
+    <row r="122" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A122" s="53">
+        <v>21</v>
+      </c>
+      <c r="B122" s="53">
+        <v>3.3669465711917415E-6</v>
+      </c>
+      <c r="C122" s="51"/>
+      <c r="D122" s="51"/>
+      <c r="E122" s="51"/>
+      <c r="F122" s="51"/>
+      <c r="G122" s="51"/>
+      <c r="H122" s="51"/>
+      <c r="I122" s="51"/>
+    </row>
+    <row r="123" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A123" s="53">
+        <v>22</v>
+      </c>
+      <c r="B123" s="53">
+        <v>5.6259478558325731E-7</v>
+      </c>
+      <c r="C123" s="51"/>
+      <c r="D123" s="51"/>
+      <c r="E123" s="51"/>
+      <c r="F123" s="51"/>
+      <c r="G123" s="51"/>
+      <c r="H123" s="51"/>
+      <c r="I123" s="51"/>
+    </row>
+    <row r="124" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A124" s="53">
+        <v>23</v>
+      </c>
+      <c r="B124" s="53">
+        <v>7.9927734387823432E-8</v>
+      </c>
+      <c r="C124" s="51"/>
+      <c r="D124" s="51"/>
+      <c r="E124" s="51"/>
+      <c r="F124" s="51"/>
+      <c r="G124" s="51"/>
+      <c r="H124" s="51"/>
+      <c r="I124" s="51"/>
+    </row>
+    <row r="125" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A125" s="53">
+        <v>24</v>
+      </c>
+      <c r="B125" s="53">
+        <v>9.5219073243709207E-9</v>
+      </c>
+      <c r="C125" s="51"/>
+      <c r="D125" s="51"/>
+      <c r="E125" s="51"/>
+      <c r="F125" s="51"/>
+      <c r="G125" s="51"/>
+      <c r="H125" s="51"/>
+      <c r="I125" s="51"/>
+    </row>
+    <row r="126" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A126" s="53">
+        <v>25</v>
+      </c>
+      <c r="B126" s="53">
+        <v>9.3341514052988687E-10</v>
+      </c>
+      <c r="C126" s="51"/>
+      <c r="D126" s="51"/>
+      <c r="E126" s="51"/>
+      <c r="F126" s="51"/>
+      <c r="G126" s="51"/>
+      <c r="H126" s="51"/>
+      <c r="I126" s="51"/>
+    </row>
+    <row r="127" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A127" s="53">
+        <v>26</v>
+      </c>
+      <c r="B127" s="53">
+        <v>7.3318090670007437E-11</v>
+      </c>
+      <c r="C127" s="51"/>
+      <c r="D127" s="51"/>
+      <c r="E127" s="51"/>
+      <c r="F127" s="51"/>
+      <c r="G127" s="51"/>
+      <c r="H127" s="51"/>
+      <c r="I127" s="51"/>
+    </row>
+    <row r="128" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A128" s="53">
+        <v>27</v>
+      </c>
+      <c r="B128" s="53">
+        <v>4.4365667802404147E-12</v>
+      </c>
+      <c r="C128" s="51"/>
+      <c r="D128" s="51"/>
+      <c r="E128" s="51"/>
+      <c r="F128" s="51"/>
+      <c r="G128" s="51"/>
+      <c r="H128" s="51"/>
+      <c r="I128" s="51"/>
+    </row>
+    <row r="129" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A129" s="53">
+        <v>28</v>
+      </c>
+      <c r="B129" s="53">
+        <v>1.9415558847128475E-13</v>
+      </c>
+      <c r="C129" s="51"/>
+      <c r="D129" s="51"/>
+      <c r="E129" s="51"/>
+      <c r="F129" s="51"/>
+      <c r="G129" s="51"/>
+      <c r="H129" s="51"/>
+      <c r="I129" s="51"/>
+    </row>
+    <row r="130" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A130" s="53">
+        <v>29</v>
+      </c>
+      <c r="B130" s="53">
+        <v>5.4691715062333685E-15</v>
+      </c>
+      <c r="C130" s="51"/>
+      <c r="D130" s="51"/>
+      <c r="E130" s="51"/>
+      <c r="F130" s="51"/>
+      <c r="G130" s="51"/>
+      <c r="H130" s="51"/>
+      <c r="I130" s="51"/>
+    </row>
+    <row r="131" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A131" s="53">
+        <v>30</v>
+      </c>
+      <c r="B131" s="53">
+        <v>7.4462898441675134E-17</v>
+      </c>
+      <c r="C131" s="51"/>
+      <c r="D131" s="51"/>
+      <c r="E131" s="51"/>
+      <c r="F131" s="51"/>
+      <c r="G131" s="51"/>
+      <c r="H131" s="51"/>
+      <c r="I131" s="51"/>
+    </row>
+    <row r="133" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A133" s="60" t="s">
+        <v>130</v>
+      </c>
+      <c r="B133" s="60"/>
+      <c r="C133" s="60"/>
+      <c r="D133" s="60"/>
+      <c r="E133" s="60"/>
+      <c r="F133" s="60"/>
+      <c r="G133" s="60"/>
+      <c r="H133" s="60"/>
+      <c r="I133" s="60"/>
+    </row>
+    <row r="134" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A134" s="55" t="s">
+        <v>214</v>
+      </c>
+      <c r="B134" s="55"/>
+      <c r="C134" s="55"/>
+      <c r="D134" s="55"/>
+      <c r="E134" s="55"/>
+      <c r="F134" s="55"/>
+      <c r="G134" s="55"/>
+      <c r="H134" s="55"/>
+      <c r="I134" s="55"/>
+    </row>
+    <row r="136" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A136" s="55" t="s">
+        <v>215</v>
+      </c>
+      <c r="B136" s="55"/>
+      <c r="C136" s="55"/>
+      <c r="D136" s="55"/>
+      <c r="E136" s="55"/>
+      <c r="F136" s="55"/>
+      <c r="G136" s="55"/>
+      <c r="H136" s="55"/>
+      <c r="I136" s="55"/>
+    </row>
+    <row r="137" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A137" s="55" t="s">
+        <v>216</v>
+      </c>
+      <c r="B137" s="57">
+        <v>29</v>
+      </c>
+      <c r="C137" s="55" t="s">
+        <v>217</v>
+      </c>
+      <c r="D137" s="55"/>
+      <c r="E137" s="55"/>
+      <c r="F137" s="55"/>
+      <c r="G137" s="55"/>
+      <c r="H137" s="55"/>
+      <c r="I137" s="55"/>
+    </row>
+    <row r="138" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A138" s="55" t="s">
+        <v>218</v>
+      </c>
+      <c r="B138" s="57">
+        <v>30</v>
+      </c>
+      <c r="C138" s="55" t="s">
+        <v>219</v>
+      </c>
+      <c r="D138" s="55"/>
+      <c r="E138" s="55"/>
+      <c r="F138" s="55"/>
+      <c r="G138" s="55"/>
+      <c r="H138" s="55"/>
+      <c r="I138" s="55"/>
+    </row>
+    <row r="139" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A139" s="55" t="s">
+        <v>220</v>
+      </c>
+      <c r="B139" s="58">
+        <v>0.96666666666666667</v>
+      </c>
+      <c r="C139" s="55" t="s">
+        <v>221</v>
+      </c>
+      <c r="D139" s="55"/>
+      <c r="E139" s="55"/>
+      <c r="F139" s="55"/>
+      <c r="G139" s="55"/>
+      <c r="H139" s="55"/>
+      <c r="I139" s="55"/>
+    </row>
+    <row r="140" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A140" s="55"/>
+      <c r="B140" s="57"/>
+      <c r="C140" s="55"/>
+      <c r="D140" s="55"/>
+      <c r="E140" s="55"/>
+      <c r="F140" s="55"/>
+      <c r="G140" s="55"/>
+      <c r="H140" s="55"/>
+      <c r="I140" s="55"/>
+    </row>
+    <row r="141" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A141" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="B141" s="58">
+        <v>0.63833848653838943</v>
+      </c>
+      <c r="C141" s="55"/>
+      <c r="D141" s="55"/>
+      <c r="E141" s="55"/>
+      <c r="F141" s="55"/>
+      <c r="G141" s="55"/>
+      <c r="H141" s="55"/>
+      <c r="I141" s="55"/>
+    </row>
+    <row r="143" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A143" s="55" t="s">
+        <v>223</v>
+      </c>
+      <c r="B143" s="55"/>
+      <c r="C143" s="55"/>
+      <c r="D143" s="55"/>
+      <c r="E143" s="55"/>
+      <c r="F143" s="55"/>
+      <c r="G143" s="55"/>
+      <c r="H143" s="55"/>
+      <c r="I143" s="55"/>
+    </row>
+    <row r="144" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A144" s="55" t="s">
+        <v>224</v>
+      </c>
+      <c r="B144" s="55"/>
+      <c r="C144" s="55"/>
+      <c r="D144" s="55"/>
+      <c r="E144" s="55"/>
+      <c r="F144" s="55"/>
+      <c r="G144" s="55"/>
+      <c r="H144" s="55"/>
+      <c r="I144" s="55"/>
+    </row>
+    <row r="146" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A146" s="59" t="s">
+        <v>225</v>
+      </c>
+      <c r="B146" s="59"/>
+      <c r="C146" s="59"/>
+      <c r="D146" s="59"/>
+      <c r="E146" s="59"/>
+      <c r="F146" s="59"/>
+      <c r="G146" s="59"/>
+      <c r="H146" s="59"/>
+      <c r="I146" s="59"/>
+    </row>
+    <row r="147" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A147" s="55" t="s">
+        <v>226</v>
+      </c>
+      <c r="B147" s="55"/>
+      <c r="C147" s="55"/>
+      <c r="D147" s="55"/>
+      <c r="E147" s="55"/>
+      <c r="F147" s="55"/>
+      <c r="G147" s="55"/>
+      <c r="H147" s="55"/>
+      <c r="I147" s="55"/>
+    </row>
+    <row r="148" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A148" s="55" t="s">
+        <v>227</v>
+      </c>
+      <c r="B148" s="55"/>
+      <c r="C148" s="55"/>
+      <c r="D148" s="55"/>
+      <c r="E148" s="55"/>
+      <c r="F148" s="55"/>
+      <c r="G148" s="55"/>
+      <c r="H148" s="55"/>
+      <c r="I148" s="55"/>
+    </row>
+    <row r="150" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A150" s="55" t="s">
+        <v>215</v>
+      </c>
+      <c r="B150" s="55"/>
+      <c r="C150" s="55"/>
+    </row>
+    <row r="151" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A151" s="55" t="s">
+        <v>216</v>
+      </c>
+      <c r="B151" s="57">
+        <v>3</v>
+      </c>
+      <c r="C151" s="55" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A152" s="55" t="s">
+        <v>229</v>
+      </c>
+      <c r="B152" s="57">
+        <v>2</v>
+      </c>
+      <c r="C152" s="55" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A154" s="55" t="s">
+        <v>231</v>
+      </c>
+      <c r="B154" s="56">
+        <v>0.18044704431548364</v>
+      </c>
+      <c r="C154" s="55"/>
+    </row>
+    <row r="156" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A156" s="55" t="s">
+        <v>232</v>
+      </c>
+      <c r="B156" s="55"/>
+      <c r="C156" s="55"/>
+    </row>
+    <row r="157" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A157" s="55" t="s">
+        <v>233</v>
+      </c>
+      <c r="B157" s="55"/>
+      <c r="C157" s="55"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10741,8 +12729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20350693-E397-43EC-A834-57A66285DFD7}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11105,7 +13093,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:N24"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>